<commit_message>
fixed asking crypto usd rate for date in future. all tsts in TestProcessorNewStruct okure
</commit_message>
<xml_diff>
--- a/test/testdata/test_ETH_SB_simplevalue_1_owner_3_deposits.xlsx
+++ b/test/testdata/test_ETH_SB_simplevalue_1_owner_3_deposits.xlsx
@@ -617,8 +617,8 @@
   </sheetPr>
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191:A221"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4392,7 +4392,7 @@
         <v>22</v>
       </c>
       <c r="I130">
-        <v>8.0215330934407802E-4</v>
+        <v>1.0633111854119191E-3</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.4">
@@ -4409,7 +4409,7 @@
         <v>22</v>
       </c>
       <c r="I131">
-        <v>8.0236279799894561E-4</v>
+        <v>1.063588877502575E-3</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.4">
@@ -4426,7 +4426,7 @@
         <v>22</v>
       </c>
       <c r="I132">
-        <v>8.0257234136293931E-4</v>
+        <v>1.0638666421147751E-3</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.4">
@@ -4443,7 +4443,7 @@
         <v>22</v>
       </c>
       <c r="I133">
-        <v>8.0278193945115817E-4</v>
+        <v>1.064144479268059E-3</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.4">
@@ -4460,7 +4460,7 @@
         <v>22</v>
       </c>
       <c r="I134">
-        <v>8.0299159227736894E-4</v>
+        <v>1.0644223889801909E-3</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.4">
@@ -4477,7 +4477,7 @@
         <v>22</v>
       </c>
       <c r="I135">
-        <v>8.0320129985578248E-4</v>
+        <v>1.064700371269822E-3</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.4">
@@ -4494,7 +4494,7 @@
         <v>22</v>
       </c>
       <c r="I136">
-        <v>8.0341106220149783E-4</v>
+        <v>1.0649784261573809E-3</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.4">
@@ -4511,7 +4511,7 @@
         <v>22</v>
       </c>
       <c r="I137">
-        <v>8.0362087932828175E-4</v>
+        <v>1.0652565536615199E-3</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.4">
@@ -4528,7 +4528,7 @@
         <v>22</v>
       </c>
       <c r="I138">
-        <v>8.0383075125034509E-4</v>
+        <v>1.0655347538008899E-3</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.4">
@@ -4545,7 +4545,7 @@
         <v>22</v>
       </c>
       <c r="I139">
-        <v>8.0404067798189871E-4</v>
+        <v>1.0658130265941419E-3</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.4">
@@ -4562,7 +4562,7 @@
         <v>22</v>
       </c>
       <c r="I140">
-        <v>8.0425065953759756E-4</v>
+        <v>1.0660913720599301E-3</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.4">
@@ -4579,7 +4579,7 @@
         <v>22</v>
       </c>
       <c r="I141">
-        <v>8.0446069593165248E-4</v>
+        <v>1.0663697902186799E-3</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.4">
@@ -4596,7 +4596,7 @@
         <v>22</v>
       </c>
       <c r="I142">
-        <v>8.0467078717827434E-4</v>
+        <v>1.0666482810881559E-3</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.4">
@@ -4613,7 +4613,7 @@
         <v>22</v>
       </c>
       <c r="I143">
-        <v>8.0488093329211807E-4</v>
+        <v>1.066926844687899E-3</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.4">
@@ -4630,7 +4630,7 @@
         <v>22</v>
       </c>
       <c r="I144">
-        <v>8.0509113428695045E-4</v>
+        <v>1.067205481036559E-3</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.4">
@@ -4647,7 +4647,7 @@
         <v>22</v>
       </c>
       <c r="I145">
-        <v>8.053013901778705E-4</v>
+        <v>1.0674841901527901E-3</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.4">
@@ -4664,7 +4664,7 @@
         <v>22</v>
       </c>
       <c r="I146">
-        <v>8.05511700978645E-4</v>
+        <v>1.0677629720570181E-3</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.4">
@@ -4681,7 +4681,7 @@
         <v>22</v>
       </c>
       <c r="I147">
-        <v>8.0572206670348478E-4</v>
+        <v>1.068041826767008E-3</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.4">
@@ -4698,7 +4698,7 @@
         <v>22</v>
       </c>
       <c r="I148">
-        <v>8.0593248736704481E-4</v>
+        <v>1.068320754302299E-3</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.4">
@@ -4715,7 +4715,7 @@
         <v>22</v>
       </c>
       <c r="I149">
-        <v>8.0614296298353594E-4</v>
+        <v>1.0685997546806549E-3</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.4">
@@ -4732,7 +4732,7 @@
         <v>22</v>
       </c>
       <c r="I150">
-        <v>8.063534935676131E-4</v>
+        <v>1.0688788279233921E-3</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.4">
@@ -4749,7 +4749,7 @@
         <v>22</v>
       </c>
       <c r="I151">
-        <v>8.0656407913348716E-4</v>
+        <v>1.069157974047386E-3</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.4">
@@ -4766,7 +4766,7 @@
         <v>22</v>
       </c>
       <c r="I152">
-        <v>8.0677471969536896E-4</v>
+        <v>1.069437193073064E-3</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.4">
@@ -4783,7 +4783,7 @@
         <v>22</v>
       </c>
       <c r="I153">
-        <v>8.0698541526746936E-4</v>
+        <v>1.069716485019079E-3</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.4">
@@ -4800,7 +4800,7 @@
         <v>22</v>
       </c>
       <c r="I154">
-        <v>8.0719616586444332E-4</v>
+        <v>1.06999584990497E-3</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.4">
@@ -4817,7 +4817,7 @@
         <v>22</v>
       </c>
       <c r="I155">
-        <v>8.0740697150094576E-4</v>
+        <v>1.0702752877485009E-3</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.4">
@@ -4834,7 +4834,7 @@
         <v>22</v>
       </c>
       <c r="I156">
-        <v>8.0761783219074346E-4</v>
+        <v>1.0705547985692121E-3</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.4">
@@ -4851,7 +4851,7 @@
         <v>22</v>
       </c>
       <c r="I157">
-        <v>8.0782874794849135E-4</v>
+        <v>1.0708343823866431E-3</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.4">
@@ -4868,7 +4868,7 @@
         <v>22</v>
       </c>
       <c r="I158">
-        <v>8.0803971878840031E-4</v>
+        <v>1.0711140392194449E-3</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.4">
@@ -4885,7 +4885,7 @@
         <v>22</v>
       </c>
       <c r="I159">
-        <v>8.0825074472512526E-4</v>
+        <v>1.0713937690871591E-3</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.4">
@@ -4902,7 +4902,7 @@
         <v>22</v>
       </c>
       <c r="I160">
-        <v>8.0846182577287706E-4</v>
+        <v>1.071673572008436E-3</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.4">
@@ -4919,7 +4919,7 @@
         <v>22</v>
       </c>
       <c r="I161">
-        <v>8.0867296194631066E-4</v>
+        <v>1.0719534480019279E-3</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.4">
@@ -4936,7 +4936,7 @@
         <v>22</v>
       </c>
       <c r="I162">
-        <v>8.0888415325963692E-4</v>
+        <v>1.0722333970880631E-3</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.4">
@@ -4953,7 +4953,7 @@
         <v>22</v>
       </c>
       <c r="I163">
-        <v>8.0909539972706668E-4</v>
+        <v>1.072513419284604E-3</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.4">
@@ -4970,7 +4970,7 @@
         <v>22</v>
       </c>
       <c r="I164">
-        <v>8.0930670136325489E-4</v>
+        <v>1.0727935146110921E-3</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.4">
@@ -4987,7 +4987,7 @@
         <v>22</v>
       </c>
       <c r="I165">
-        <v>8.095180581824124E-4</v>
+        <v>1.0730736830870671E-3</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.4">
@@ -5004,7 +5004,7 @@
         <v>22</v>
       </c>
       <c r="I166">
-        <v>8.0972947019919417E-4</v>
+        <v>1.0733539247311801E-3</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.4">
@@ -5021,7 +5021,7 @@
         <v>22</v>
       </c>
       <c r="I167">
-        <v>8.0994093742781104E-4</v>
+        <v>1.0736342395620819E-3</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.4">
@@ -5038,7 +5038,7 @@
         <v>22</v>
       </c>
       <c r="I168">
-        <v>8.1015245988247386E-4</v>
+        <v>1.073914627599315E-3</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.4">
@@ -5055,7 +5055,7 @@
         <v>22</v>
       </c>
       <c r="I169">
-        <v>8.1036403757828168E-4</v>
+        <v>1.074195088863306E-3</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.4">
@@ -5072,7 +5072,7 @@
         <v>22</v>
       </c>
       <c r="I170">
-        <v>8.1057567052900126E-4</v>
+        <v>1.07447562337093E-3</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.4">
@@ -5089,7 +5089,7 @@
         <v>22</v>
       </c>
       <c r="I171">
-        <v>8.1078735874973162E-4</v>
+        <v>1.0747562311426151E-3</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.4">
@@ -5106,7 +5106,7 @@
         <v>22</v>
       </c>
       <c r="I172">
-        <v>8.1099910225423955E-4</v>
+        <v>1.075036912197014E-3</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.4">
@@ -5123,7 +5123,7 @@
         <v>22</v>
       </c>
       <c r="I173">
-        <v>8.1121090105717997E-4</v>
+        <v>1.0753176665536661E-3</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.4">
@@ -5140,7 +5140,7 @@
         <v>22</v>
       </c>
       <c r="I174">
-        <v>8.1142275517320783E-4</v>
+        <v>1.075598494231222E-3</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.4">
@@ -5157,7 +5157,7 @@
         <v>22</v>
       </c>
       <c r="I175">
-        <v>8.11634664616534E-4</v>
+        <v>1.075879395250112E-3</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.4">
@@ -5174,7 +5174,7 @@
         <v>22</v>
       </c>
       <c r="I176">
-        <v>8.118466294018134E-4</v>
+        <v>1.076160369628099E-3</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.4">
@@ -5191,7 +5191,7 @@
         <v>22</v>
       </c>
       <c r="I177">
-        <v>8.1205864954325691E-4</v>
+        <v>1.076441417383833E-3</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.4">
@@ -5208,7 +5208,7 @@
         <v>22</v>
       </c>
       <c r="I178">
-        <v>8.1227072505551945E-4</v>
+        <v>1.076722538538633E-3</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.4">
@@ -5225,7 +5225,7 @@
         <v>22</v>
       </c>
       <c r="I179">
-        <v>8.1248285595281189E-4</v>
+        <v>1.077003733109372E-3</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.4">
@@ -5242,7 +5242,7 @@
         <v>22</v>
       </c>
       <c r="I180">
-        <v>8.1269504224978917E-4</v>
+        <v>1.0772850011173669E-3</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.4">
@@ -5259,7 +5259,7 @@
         <v>22</v>
       </c>
       <c r="I181">
-        <v>8.1290728396066214E-4</v>
+        <v>1.077566342580383E-3</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.4">
@@ -5276,7 +5276,7 @@
         <v>22</v>
       </c>
       <c r="I182">
-        <v>8.1311958110052984E-4</v>
+        <v>1.07784775751707E-3</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.4">
@@ -5293,7 +5293,7 @@
         <v>22</v>
       </c>
       <c r="I183">
-        <v>8.1333193368315904E-4</v>
+        <v>1.078129245948745E-3</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.4">
@@ -5310,7 +5310,7 @@
         <v>22</v>
       </c>
       <c r="I184">
-        <v>8.1354434172364876E-4</v>
+        <v>1.0784108078922829E-3</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.4">
@@ -5327,7 +5327,7 @@
         <v>22</v>
       </c>
       <c r="I185">
-        <v>8.1375680523620986E-4</v>
+        <v>1.078692443368112E-3</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.4">
@@ -5344,7 +5344,7 @@
         <v>22</v>
       </c>
       <c r="I186">
-        <v>8.1396932423505319E-4</v>
+        <v>1.078974152395773E-3</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.4">
@@ -5361,7 +5361,7 @@
         <v>22</v>
       </c>
       <c r="I187">
-        <v>8.1418189873483371E-4</v>
+        <v>1.079255934993917E-3</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.4">
@@ -5378,7 +5378,7 @@
         <v>22</v>
       </c>
       <c r="I188">
-        <v>8.1439452875020635E-4</v>
+        <v>1.079537791181195E-3</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.4">
@@ -5395,7 +5395,7 @@
         <v>22</v>
       </c>
       <c r="I189">
-        <v>8.1460721429582605E-4</v>
+        <v>1.0798197209780369E-3</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.4">
@@ -5412,7 +5412,7 @@
         <v>22</v>
       </c>
       <c r="I190">
-        <v>8.1481995538545959E-4</v>
+        <v>1.080101724403093E-3</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.4">
@@ -5429,7 +5429,7 @@
         <v>22</v>
       </c>
       <c r="I191">
-        <v>1.076190628102047E-3</v>
+        <v>1.080383801475016E-3</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.4">
@@ -5446,7 +5446,7 @@
         <v>22</v>
       </c>
       <c r="I192">
-        <v>1.0764716837607931E-3</v>
+        <v>1.080665952214233E-3</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.4">
@@ -5463,7 +5463,7 @@
         <v>22</v>
       </c>
       <c r="I193">
-        <v>1.076752812819493E-3</v>
+        <v>1.080948176639396E-3</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.4">
@@ -5480,7 +5480,7 @@
         <v>22</v>
       </c>
       <c r="I194">
-        <v>1.0770340152967961E-3</v>
+        <v>1.081230474769157E-3</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.4">
@@ -5497,7 +5497,7 @@
         <v>22</v>
       </c>
       <c r="I195">
-        <v>1.0773152912131321E-3</v>
+        <v>1.0815128466230559E-3</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.4">
@@ -5514,7 +5514,7 @@
         <v>22</v>
       </c>
       <c r="I196">
-        <v>1.0775966405862649E-3</v>
+        <v>1.081795292221521E-3</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.4">
@@ -5531,7 +5531,7 @@
         <v>22</v>
       </c>
       <c r="I197">
-        <v>1.077878063436621E-3</v>
+        <v>1.082077811582316E-3</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.4">
@@ -5548,7 +5548,7 @@
         <v>22</v>
       </c>
       <c r="I198">
-        <v>1.078159559781966E-3</v>
+        <v>1.08236040472498E-3</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.4">
@@ -5565,7 +5565,7 @@
         <v>22</v>
       </c>
       <c r="I199">
-        <v>1.078441129642727E-3</v>
+        <v>1.082643071669942E-3</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.4">
@@ -5582,7 +5582,7 @@
         <v>22</v>
       </c>
       <c r="I200">
-        <v>1.078722773037555E-3</v>
+        <v>1.082925812434965E-3</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.4">
@@ -5599,7 +5599,7 @@
         <v>22</v>
       </c>
       <c r="I201">
-        <v>1.079004489985991E-3</v>
+        <v>1.0832086270395891E-3</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.4">
@@ -5616,7 +5616,7 @@
         <v>22</v>
       </c>
       <c r="I202">
-        <v>1.0792862805066861E-3</v>
+        <v>1.083491515504242E-3</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.4">
@@ -5633,7 +5633,7 @@
         <v>22</v>
       </c>
       <c r="I203">
-        <v>1.0795681446191809E-3</v>
+        <v>1.0837744778475771E-3</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.4">
@@ -5650,7 +5650,7 @@
         <v>22</v>
       </c>
       <c r="I204">
-        <v>1.079850082343015E-3</v>
+        <v>1.084057514088244E-3</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.4">
@@ -5667,7 +5667,7 @@
         <v>22</v>
       </c>
       <c r="I205">
-        <v>1.0801320936968391E-3</v>
+        <v>1.0843406242457829E-3</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.4">
@@ -5684,7 +5684,7 @@
         <v>22</v>
       </c>
       <c r="I206">
-        <v>1.0804141787001951E-3</v>
+        <v>1.084623808340623E-3</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.4">
@@ -5701,7 +5701,7 @@
         <v>22</v>
       </c>
       <c r="I207">
-        <v>1.0806963373726219E-3</v>
+        <v>1.084907066390528E-3</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.4">
@@ -5718,7 +5718,7 @@
         <v>22</v>
       </c>
       <c r="I208">
-        <v>1.080978569732771E-3</v>
+        <v>1.085190398415925E-3</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.4">
@@ -5735,7 +5735,7 @@
         <v>22</v>
       </c>
       <c r="I209">
-        <v>1.0812608758001829E-3</v>
+        <v>1.0854738044354659E-3</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.4">
@@ -5752,7 +5752,7 @@
         <v>22</v>
       </c>
       <c r="I210">
-        <v>1.0815432555943969E-3</v>
+        <v>1.0857572844686909E-3</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.4">
@@ -5769,7 +5769,7 @@
         <v>22</v>
       </c>
       <c r="I211">
-        <v>1.0818257091331769E-3</v>
+        <v>1.086040838535141E-3</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.4">
@@ -5786,7 +5786,7 @@
         <v>22</v>
       </c>
       <c r="I212">
-        <v>1.08210823643784E-3</v>
+        <v>1.0863244666534651E-3</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.4">
@@ -5803,7 +5803,7 @@
         <v>22</v>
       </c>
       <c r="I213">
-        <v>1.0823908375270359E-3</v>
+        <v>1.0866081688440941E-3</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.4">
@@ -5820,7 +5820,7 @@
         <v>22</v>
       </c>
       <c r="I214">
-        <v>1.0826735124185301E-3</v>
+        <v>1.0868919451256791E-3</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.4">
@@ -5837,7 +5837,7 @@
         <v>22</v>
       </c>
       <c r="I215">
-        <v>1.082956261133639E-3</v>
+        <v>1.087175795517759E-3</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.4">
@@ -5854,7 +5854,7 @@
         <v>22</v>
       </c>
       <c r="I216">
-        <v>1.083239083691012E-3</v>
+        <v>1.0874597200389859E-3</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.4">
@@ -5871,7 +5871,7 @@
         <v>22</v>
       </c>
       <c r="I217">
-        <v>1.083521980109303E-3</v>
+        <v>1.087743718709788E-3</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.4">
@@ -5888,7 +5888,7 @@
         <v>22</v>
       </c>
       <c r="I218">
-        <v>1.083804950408052E-3</v>
+        <v>1.0880277915488179E-3</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.4">
@@ -5905,7 +5905,7 @@
         <v>22</v>
       </c>
       <c r="I219">
-        <v>1.0840879946076849E-3</v>
+        <v>1.088311938576503E-3</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.4">
@@ -5922,7 +5922,7 @@
         <v>22</v>
       </c>
       <c r="I220">
-        <v>1.0843711127250799E-3</v>
+        <v>1.088596159810606E-3</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.4">
@@ -5939,7 +5939,7 @@
         <v>22</v>
       </c>
       <c r="I221">
-        <v>1.08465430478244E-3</v>
+        <v>1.088880455271557E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>